<commit_message>
attempt at adding decommissioning option
</commit_message>
<xml_diff>
--- a/input_data/fuels.xlsx
+++ b/input_data/fuels.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mscle\Desktop\global_shipping_model\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mscle\Desktop\global_shipping_model\input_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="100">
   <si>
     <t>Hydrogen</t>
   </si>
@@ -551,6 +551,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -566,7 +567,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1945,7 +1945,7 @@
   <dimension ref="B2:BQ87"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D78" sqref="D78"/>
+      <selection activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1967,18 +1967,18 @@
     <row r="5" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C5" s="10"/>
       <c r="D5" s="11"/>
-      <c r="E5" s="54" t="s">
+      <c r="E5" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
-      <c r="I5" s="54" t="s">
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="J5" s="54"/>
-      <c r="K5" s="54"/>
-      <c r="L5" s="56"/>
+      <c r="J5" s="55"/>
+      <c r="K5" s="55"/>
+      <c r="L5" s="57"/>
     </row>
     <row r="6" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C6" s="12" t="s">
@@ -1987,38 +1987,38 @@
       <c r="D6" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="E6" s="57">
+      <c r="E6" s="58">
         <v>30</v>
       </c>
-      <c r="F6" s="57"/>
-      <c r="G6" s="57"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57">
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="58"/>
+      <c r="I6" s="58">
         <v>20</v>
       </c>
-      <c r="J6" s="57"/>
-      <c r="K6" s="57"/>
-      <c r="L6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
+      <c r="L6" s="59"/>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C7" s="16"/>
       <c r="D7" s="13"/>
-      <c r="E7" s="57" t="s">
+      <c r="E7" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="57"/>
-      <c r="G7" s="57" t="s">
+      <c r="F7" s="58"/>
+      <c r="G7" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="H7" s="57"/>
-      <c r="I7" s="57" t="s">
+      <c r="H7" s="58"/>
+      <c r="I7" s="58" t="s">
         <v>59</v>
       </c>
-      <c r="J7" s="57"/>
-      <c r="K7" s="57" t="s">
+      <c r="J7" s="58"/>
+      <c r="K7" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="L7" s="58"/>
+      <c r="L7" s="59"/>
     </row>
     <row r="8" spans="3:14" x14ac:dyDescent="0.25">
       <c r="C8" s="16"/>
@@ -2297,18 +2297,18 @@
       <c r="D25" s="51" t="s">
         <v>96</v>
       </c>
-      <c r="E25" s="54" t="s">
+      <c r="E25" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="F25" s="54"/>
-      <c r="G25" s="55" t="s">
+      <c r="F25" s="55"/>
+      <c r="G25" s="56" t="s">
         <v>94</v>
       </c>
-      <c r="H25" s="55"/>
-      <c r="I25" s="54" t="s">
+      <c r="H25" s="56"/>
+      <c r="I25" s="55" t="s">
         <v>95</v>
       </c>
-      <c r="J25" s="56"/>
+      <c r="J25" s="57"/>
     </row>
     <row r="26" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C26" s="16"/>
@@ -8465,2621 +8465,2651 @@
       <c r="C78" s="34">
         <v>1000</v>
       </c>
-      <c r="E78" s="59">
+      <c r="D78" t="s">
+        <v>8</v>
+      </c>
+      <c r="E78" s="54">
         <f>+E66*$C$78</f>
         <v>5.8805693069306928</v>
       </c>
-      <c r="F78" s="59">
+      <c r="F78" s="54">
         <f t="shared" ref="F78:BQ82" si="90">+F66*$C$78</f>
         <v>5.8805693069306928</v>
       </c>
-      <c r="G78" s="59">
+      <c r="G78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="H78" s="59">
+      <c r="H78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="I78" s="59">
+      <c r="I78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="J78" s="59">
+      <c r="J78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="K78" s="59">
+      <c r="K78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="L78" s="59">
+      <c r="L78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="M78" s="59">
+      <c r="M78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="N78" s="59">
+      <c r="N78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="O78" s="59">
+      <c r="O78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="P78" s="59">
+      <c r="P78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="Q78" s="59">
+      <c r="Q78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="R78" s="59">
+      <c r="R78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="S78" s="59">
+      <c r="S78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="T78" s="59">
+      <c r="T78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="U78" s="59">
+      <c r="U78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="V78" s="59">
+      <c r="V78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="W78" s="59">
+      <c r="W78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="X78" s="59">
+      <c r="X78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="Y78" s="59">
+      <c r="Y78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="Z78" s="59">
+      <c r="Z78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="AA78" s="59">
+      <c r="AA78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="AB78" s="59">
+      <c r="AB78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="AC78" s="59">
+      <c r="AC78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="AD78" s="59">
+      <c r="AD78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="AE78" s="59">
+      <c r="AE78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="AF78" s="59">
+      <c r="AF78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="AG78" s="59">
+      <c r="AG78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="AH78" s="59">
+      <c r="AH78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="AI78" s="59">
+      <c r="AI78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="AJ78" s="59">
+      <c r="AJ78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="AK78" s="59">
+      <c r="AK78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="AL78" s="59">
+      <c r="AL78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="AM78" s="59">
+      <c r="AM78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="AN78" s="59">
+      <c r="AN78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="AO78" s="59">
+      <c r="AO78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="AP78" s="59">
+      <c r="AP78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="AQ78" s="59">
+      <c r="AQ78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="AR78" s="59">
+      <c r="AR78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="AS78" s="59">
+      <c r="AS78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="AT78" s="59">
+      <c r="AT78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="AU78" s="59">
+      <c r="AU78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="AV78" s="59">
+      <c r="AV78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="AW78" s="59">
+      <c r="AW78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="AX78" s="59">
+      <c r="AX78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="AY78" s="59">
+      <c r="AY78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="AZ78" s="59">
+      <c r="AZ78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="BA78" s="59">
+      <c r="BA78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="BB78" s="59">
+      <c r="BB78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="BC78" s="59">
+      <c r="BC78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="BD78" s="59">
+      <c r="BD78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="BE78" s="59">
+      <c r="BE78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="BF78" s="59">
+      <c r="BF78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="BG78" s="59">
+      <c r="BG78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="BH78" s="59">
+      <c r="BH78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="BI78" s="59">
+      <c r="BI78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="BJ78" s="59">
+      <c r="BJ78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="BK78" s="59">
+      <c r="BK78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="BL78" s="59">
+      <c r="BL78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="BM78" s="59">
+      <c r="BM78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="BN78" s="59">
+      <c r="BN78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="BO78" s="59">
+      <c r="BO78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="BP78" s="59">
+      <c r="BP78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
-      <c r="BQ78" s="59">
+      <c r="BQ78" s="54">
         <f t="shared" si="90"/>
         <v>5.8805693069306928</v>
       </c>
     </row>
     <row r="79" spans="3:69" x14ac:dyDescent="0.25">
-      <c r="E79" s="59">
+      <c r="D79" t="s">
+        <v>42</v>
+      </c>
+      <c r="E79" s="54">
         <f t="shared" ref="E79:T87" si="91">+E67*$C$78</f>
         <v>12.750000000000002</v>
       </c>
-      <c r="F79" s="59">
+      <c r="F79" s="54">
         <f t="shared" si="91"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="G79" s="59">
+      <c r="G79" s="54">
         <f t="shared" si="91"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="H79" s="59">
+      <c r="H79" s="54">
         <f t="shared" si="91"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="I79" s="59">
+      <c r="I79" s="54">
         <f t="shared" si="91"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="J79" s="59">
+      <c r="J79" s="54">
         <f t="shared" si="91"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="K79" s="59">
+      <c r="K79" s="54">
         <f t="shared" si="91"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="L79" s="59">
+      <c r="L79" s="54">
         <f t="shared" si="91"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="M79" s="59">
+      <c r="M79" s="54">
         <f t="shared" si="91"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="N79" s="59">
+      <c r="N79" s="54">
         <f t="shared" si="91"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="O79" s="59">
+      <c r="O79" s="54">
         <f t="shared" si="91"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="P79" s="59">
+      <c r="P79" s="54">
         <f t="shared" si="91"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="Q79" s="59">
+      <c r="Q79" s="54">
         <f t="shared" si="91"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="R79" s="59">
+      <c r="R79" s="54">
         <f t="shared" si="91"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="S79" s="59">
+      <c r="S79" s="54">
         <f t="shared" si="91"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="T79" s="59">
+      <c r="T79" s="54">
         <f t="shared" si="91"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="U79" s="59">
+      <c r="U79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="V79" s="59">
+      <c r="V79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="W79" s="59">
+      <c r="W79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="X79" s="59">
+      <c r="X79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="Y79" s="59">
+      <c r="Y79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="Z79" s="59">
+      <c r="Z79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="AA79" s="59">
+      <c r="AA79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="AB79" s="59">
+      <c r="AB79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="AC79" s="59">
+      <c r="AC79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="AD79" s="59">
+      <c r="AD79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="AE79" s="59">
+      <c r="AE79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="AF79" s="59">
+      <c r="AF79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="AG79" s="59">
+      <c r="AG79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="AH79" s="59">
+      <c r="AH79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="AI79" s="59">
+      <c r="AI79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="AJ79" s="59">
+      <c r="AJ79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="AK79" s="59">
+      <c r="AK79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="AL79" s="59">
+      <c r="AL79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="AM79" s="59">
+      <c r="AM79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="AN79" s="59">
+      <c r="AN79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="AO79" s="59">
+      <c r="AO79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="AP79" s="59">
+      <c r="AP79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="AQ79" s="59">
+      <c r="AQ79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="AR79" s="59">
+      <c r="AR79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="AS79" s="59">
+      <c r="AS79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="AT79" s="59">
+      <c r="AT79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="AU79" s="59">
+      <c r="AU79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="AV79" s="59">
+      <c r="AV79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="AW79" s="59">
+      <c r="AW79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="AX79" s="59">
+      <c r="AX79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="AY79" s="59">
+      <c r="AY79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="AZ79" s="59">
+      <c r="AZ79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="BA79" s="59">
+      <c r="BA79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="BB79" s="59">
+      <c r="BB79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="BC79" s="59">
+      <c r="BC79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="BD79" s="59">
+      <c r="BD79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="BE79" s="59">
+      <c r="BE79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="BF79" s="59">
+      <c r="BF79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="BG79" s="59">
+      <c r="BG79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="BH79" s="59">
+      <c r="BH79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="BI79" s="59">
+      <c r="BI79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="BJ79" s="59">
+      <c r="BJ79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="BK79" s="59">
+      <c r="BK79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="BL79" s="59">
+      <c r="BL79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="BM79" s="59">
+      <c r="BM79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="BN79" s="59">
+      <c r="BN79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="BO79" s="59">
+      <c r="BO79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="BP79" s="59">
+      <c r="BP79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
-      <c r="BQ79" s="59">
+      <c r="BQ79" s="54">
         <f t="shared" si="90"/>
         <v>12.750000000000002</v>
       </c>
     </row>
     <row r="80" spans="3:69" x14ac:dyDescent="0.25">
-      <c r="E80" s="59">
+      <c r="D80" t="s">
+        <v>7</v>
+      </c>
+      <c r="E80" s="54">
         <f t="shared" si="91"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="F80" s="59">
+      <c r="F80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="G80" s="59">
+      <c r="G80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="H80" s="59">
+      <c r="H80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="I80" s="59">
+      <c r="I80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="J80" s="59">
+      <c r="J80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="K80" s="59">
+      <c r="K80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="L80" s="59">
+      <c r="L80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="M80" s="59">
+      <c r="M80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="N80" s="59">
+      <c r="N80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="O80" s="59">
+      <c r="O80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="P80" s="59">
+      <c r="P80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="Q80" s="59">
+      <c r="Q80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="R80" s="59">
+      <c r="R80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="S80" s="59">
+      <c r="S80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="T80" s="59">
+      <c r="T80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="U80" s="59">
+      <c r="U80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="V80" s="59">
+      <c r="V80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="W80" s="59">
+      <c r="W80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="X80" s="59">
+      <c r="X80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="Y80" s="59">
+      <c r="Y80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="Z80" s="59">
+      <c r="Z80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="AA80" s="59">
+      <c r="AA80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="AB80" s="59">
+      <c r="AB80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="AC80" s="59">
+      <c r="AC80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="AD80" s="59">
+      <c r="AD80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="AE80" s="59">
+      <c r="AE80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="AF80" s="59">
+      <c r="AF80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="AG80" s="59">
+      <c r="AG80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="AH80" s="59">
+      <c r="AH80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="AI80" s="59">
+      <c r="AI80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="AJ80" s="59">
+      <c r="AJ80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="AK80" s="59">
+      <c r="AK80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="AL80" s="59">
+      <c r="AL80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="AM80" s="59">
+      <c r="AM80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="AN80" s="59">
+      <c r="AN80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="AO80" s="59">
+      <c r="AO80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="AP80" s="59">
+      <c r="AP80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="AQ80" s="59">
+      <c r="AQ80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="AR80" s="59">
+      <c r="AR80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="AS80" s="59">
+      <c r="AS80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="AT80" s="59">
+      <c r="AT80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="AU80" s="59">
+      <c r="AU80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="AV80" s="59">
+      <c r="AV80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="AW80" s="59">
+      <c r="AW80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="AX80" s="59">
+      <c r="AX80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="AY80" s="59">
+      <c r="AY80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="AZ80" s="59">
+      <c r="AZ80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="BA80" s="59">
+      <c r="BA80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="BB80" s="59">
+      <c r="BB80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="BC80" s="59">
+      <c r="BC80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="BD80" s="59">
+      <c r="BD80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="BE80" s="59">
+      <c r="BE80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="BF80" s="59">
+      <c r="BF80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="BG80" s="59">
+      <c r="BG80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="BH80" s="59">
+      <c r="BH80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="BI80" s="59">
+      <c r="BI80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="BJ80" s="59">
+      <c r="BJ80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="BK80" s="59">
+      <c r="BK80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="BL80" s="59">
+      <c r="BL80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="BM80" s="59">
+      <c r="BM80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="BN80" s="59">
+      <c r="BN80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="BO80" s="59">
+      <c r="BO80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="BP80" s="59">
+      <c r="BP80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
-      <c r="BQ80" s="59">
+      <c r="BQ80" s="54">
         <f t="shared" si="90"/>
         <v>6.2726072607260726</v>
       </c>
     </row>
-    <row r="81" spans="5:69" x14ac:dyDescent="0.25">
-      <c r="E81" s="59">
+    <row r="81" spans="4:69" x14ac:dyDescent="0.25">
+      <c r="D81" t="s">
+        <v>1</v>
+      </c>
+      <c r="E81" s="54">
         <f t="shared" si="91"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="F81" s="59">
+      <c r="F81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="G81" s="59">
+      <c r="G81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="H81" s="59">
+      <c r="H81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="I81" s="59">
+      <c r="I81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="J81" s="59">
+      <c r="J81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="K81" s="59">
+      <c r="K81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="L81" s="59">
+      <c r="L81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="M81" s="59">
+      <c r="M81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="N81" s="59">
+      <c r="N81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="O81" s="59">
+      <c r="O81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="P81" s="59">
+      <c r="P81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="Q81" s="59">
+      <c r="Q81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="R81" s="59">
+      <c r="R81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="S81" s="59">
+      <c r="S81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="T81" s="59">
+      <c r="T81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="U81" s="59">
+      <c r="U81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="V81" s="59">
+      <c r="V81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="W81" s="59">
+      <c r="W81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="X81" s="59">
+      <c r="X81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="Y81" s="59">
+      <c r="Y81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="Z81" s="59">
+      <c r="Z81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="AA81" s="59">
+      <c r="AA81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="AB81" s="59">
+      <c r="AB81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="AC81" s="59">
+      <c r="AC81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="AD81" s="59">
+      <c r="AD81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="AE81" s="59">
+      <c r="AE81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="AF81" s="59">
+      <c r="AF81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="AG81" s="59">
+      <c r="AG81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="AH81" s="59">
+      <c r="AH81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="AI81" s="59">
+      <c r="AI81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="AJ81" s="59">
+      <c r="AJ81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="AK81" s="59">
+      <c r="AK81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="AL81" s="59">
+      <c r="AL81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="AM81" s="59">
+      <c r="AM81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="AN81" s="59">
+      <c r="AN81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="AO81" s="59">
+      <c r="AO81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="AP81" s="59">
+      <c r="AP81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="AQ81" s="59">
+      <c r="AQ81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="AR81" s="59">
+      <c r="AR81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="AS81" s="59">
+      <c r="AS81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="AT81" s="59">
+      <c r="AT81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="AU81" s="59">
+      <c r="AU81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="AV81" s="59">
+      <c r="AV81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="AW81" s="59">
+      <c r="AW81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="AX81" s="59">
+      <c r="AX81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="AY81" s="59">
+      <c r="AY81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="AZ81" s="59">
+      <c r="AZ81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="BA81" s="59">
+      <c r="BA81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="BB81" s="59">
+      <c r="BB81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="BC81" s="59">
+      <c r="BC81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="BD81" s="59">
+      <c r="BD81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="BE81" s="59">
+      <c r="BE81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="BF81" s="59">
+      <c r="BF81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="BG81" s="59">
+      <c r="BG81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="BH81" s="59">
+      <c r="BH81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="BI81" s="59">
+      <c r="BI81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="BJ81" s="59">
+      <c r="BJ81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="BK81" s="59">
+      <c r="BK81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="BL81" s="59">
+      <c r="BL81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="BM81" s="59">
+      <c r="BM81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="BN81" s="59">
+      <c r="BN81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="BO81" s="59">
+      <c r="BO81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="BP81" s="59">
+      <c r="BP81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
-      <c r="BQ81" s="59">
+      <c r="BQ81" s="54">
         <f t="shared" si="90"/>
         <v>7.0566831683168312</v>
       </c>
     </row>
-    <row r="82" spans="5:69" x14ac:dyDescent="0.25">
-      <c r="E82" s="59">
+    <row r="82" spans="4:69" x14ac:dyDescent="0.25">
+      <c r="D82" t="s">
+        <v>13</v>
+      </c>
+      <c r="E82" s="54">
         <f t="shared" si="91"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="F82" s="59">
+      <c r="F82" s="54">
         <f t="shared" si="90"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="G82" s="59">
+      <c r="G82" s="54">
         <f t="shared" si="90"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="H82" s="59">
+      <c r="H82" s="54">
         <f t="shared" si="90"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="I82" s="59">
+      <c r="I82" s="54">
         <f t="shared" si="90"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="J82" s="59">
+      <c r="J82" s="54">
         <f t="shared" si="90"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="K82" s="59">
+      <c r="K82" s="54">
         <f t="shared" si="90"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="L82" s="59">
+      <c r="L82" s="54">
         <f t="shared" si="90"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="M82" s="59">
+      <c r="M82" s="54">
         <f t="shared" si="90"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="N82" s="59">
+      <c r="N82" s="54">
         <f t="shared" si="90"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="O82" s="59">
+      <c r="O82" s="54">
         <f t="shared" si="90"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="P82" s="59">
+      <c r="P82" s="54">
         <f t="shared" si="90"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="Q82" s="59">
+      <c r="Q82" s="54">
         <f t="shared" si="90"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="R82" s="59">
+      <c r="R82" s="54">
         <f t="shared" si="90"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="S82" s="59">
+      <c r="S82" s="54">
         <f t="shared" si="90"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="T82" s="59">
+      <c r="T82" s="54">
         <f t="shared" ref="F82:BQ86" si="92">+T70*$C$78</f>
         <v>9.4089108910891088</v>
       </c>
-      <c r="U82" s="59">
+      <c r="U82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="V82" s="59">
+      <c r="V82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="W82" s="59">
+      <c r="W82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="X82" s="59">
+      <c r="X82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="Y82" s="59">
+      <c r="Y82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="Z82" s="59">
+      <c r="Z82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="AA82" s="59">
+      <c r="AA82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="AB82" s="59">
+      <c r="AB82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="AC82" s="59">
+      <c r="AC82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="AD82" s="59">
+      <c r="AD82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="AE82" s="59">
+      <c r="AE82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="AF82" s="59">
+      <c r="AF82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="AG82" s="59">
+      <c r="AG82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="AH82" s="59">
+      <c r="AH82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="AI82" s="59">
+      <c r="AI82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="AJ82" s="59">
+      <c r="AJ82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="AK82" s="59">
+      <c r="AK82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="AL82" s="59">
+      <c r="AL82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="AM82" s="59">
+      <c r="AM82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="AN82" s="59">
+      <c r="AN82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="AO82" s="59">
+      <c r="AO82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="AP82" s="59">
+      <c r="AP82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="AQ82" s="59">
+      <c r="AQ82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="AR82" s="59">
+      <c r="AR82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="AS82" s="59">
+      <c r="AS82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="AT82" s="59">
+      <c r="AT82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="AU82" s="59">
+      <c r="AU82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="AV82" s="59">
+      <c r="AV82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="AW82" s="59">
+      <c r="AW82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="AX82" s="59">
+      <c r="AX82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="AY82" s="59">
+      <c r="AY82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="AZ82" s="59">
+      <c r="AZ82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="BA82" s="59">
+      <c r="BA82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="BB82" s="59">
+      <c r="BB82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="BC82" s="59">
+      <c r="BC82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="BD82" s="59">
+      <c r="BD82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="BE82" s="59">
+      <c r="BE82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="BF82" s="59">
+      <c r="BF82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="BG82" s="59">
+      <c r="BG82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="BH82" s="59">
+      <c r="BH82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="BI82" s="59">
+      <c r="BI82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="BJ82" s="59">
+      <c r="BJ82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="BK82" s="59">
+      <c r="BK82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="BL82" s="59">
+      <c r="BL82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="BM82" s="59">
+      <c r="BM82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="BN82" s="59">
+      <c r="BN82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="BO82" s="59">
+      <c r="BO82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="BP82" s="59">
+      <c r="BP82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
-      <c r="BQ82" s="59">
+      <c r="BQ82" s="54">
         <f t="shared" si="92"/>
         <v>9.4089108910891088</v>
       </c>
     </row>
-    <row r="83" spans="5:69" x14ac:dyDescent="0.25">
-      <c r="E83" s="59">
+    <row r="83" spans="4:69" x14ac:dyDescent="0.25">
+      <c r="D83" t="s">
+        <v>43</v>
+      </c>
+      <c r="E83" s="54">
         <f t="shared" si="91"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="F83" s="59">
+      <c r="F83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="G83" s="59">
+      <c r="G83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="H83" s="59">
+      <c r="H83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="I83" s="59">
+      <c r="I83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="J83" s="59">
+      <c r="J83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="K83" s="59">
+      <c r="K83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="L83" s="59">
+      <c r="L83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="M83" s="59">
+      <c r="M83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="N83" s="59">
+      <c r="N83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="O83" s="59">
+      <c r="O83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="P83" s="59">
+      <c r="P83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="Q83" s="59">
+      <c r="Q83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="R83" s="59">
+      <c r="R83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="S83" s="59">
+      <c r="S83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="T83" s="59">
+      <c r="T83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="U83" s="59">
+      <c r="U83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="V83" s="59">
+      <c r="V83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="W83" s="59">
+      <c r="W83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="X83" s="59">
+      <c r="X83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="Y83" s="59">
+      <c r="Y83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="Z83" s="59">
+      <c r="Z83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="AA83" s="59">
+      <c r="AA83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="AB83" s="59">
+      <c r="AB83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="AC83" s="59">
+      <c r="AC83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="AD83" s="59">
+      <c r="AD83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="AE83" s="59">
+      <c r="AE83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="AF83" s="59">
+      <c r="AF83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="AG83" s="59">
+      <c r="AG83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="AH83" s="59">
+      <c r="AH83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="AI83" s="59">
+      <c r="AI83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="AJ83" s="59">
+      <c r="AJ83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="AK83" s="59">
+      <c r="AK83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="AL83" s="59">
+      <c r="AL83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="AM83" s="59">
+      <c r="AM83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="AN83" s="59">
+      <c r="AN83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="AO83" s="59">
+      <c r="AO83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="AP83" s="59">
+      <c r="AP83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="AQ83" s="59">
+      <c r="AQ83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="AR83" s="59">
+      <c r="AR83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="AS83" s="59">
+      <c r="AS83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="AT83" s="59">
+      <c r="AT83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="AU83" s="59">
+      <c r="AU83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="AV83" s="59">
+      <c r="AV83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="AW83" s="59">
+      <c r="AW83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="AX83" s="59">
+      <c r="AX83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="AY83" s="59">
+      <c r="AY83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="AZ83" s="59">
+      <c r="AZ83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="BA83" s="59">
+      <c r="BA83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="BB83" s="59">
+      <c r="BB83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="BC83" s="59">
+      <c r="BC83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="BD83" s="59">
+      <c r="BD83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="BE83" s="59">
+      <c r="BE83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="BF83" s="59">
+      <c r="BF83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="BG83" s="59">
+      <c r="BG83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="BH83" s="59">
+      <c r="BH83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="BI83" s="59">
+      <c r="BI83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="BJ83" s="59">
+      <c r="BJ83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="BK83" s="59">
+      <c r="BK83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="BL83" s="59">
+      <c r="BL83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="BM83" s="59">
+      <c r="BM83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="BN83" s="59">
+      <c r="BN83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="BO83" s="59">
+      <c r="BO83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="BP83" s="59">
+      <c r="BP83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
-      <c r="BQ83" s="59">
+      <c r="BQ83" s="54">
         <f t="shared" si="92"/>
         <v>10.624999999999998</v>
       </c>
     </row>
-    <row r="84" spans="5:69" x14ac:dyDescent="0.25">
-      <c r="E84" s="59">
+    <row r="84" spans="4:69" x14ac:dyDescent="0.25">
+      <c r="D84" t="s">
+        <v>44</v>
+      </c>
+      <c r="E84" s="54">
         <f t="shared" si="91"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="F84" s="59">
+      <c r="F84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="G84" s="59">
+      <c r="G84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="H84" s="59">
+      <c r="H84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="I84" s="59">
+      <c r="I84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="J84" s="59">
+      <c r="J84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="K84" s="59">
+      <c r="K84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="L84" s="59">
+      <c r="L84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="M84" s="59">
+      <c r="M84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="N84" s="59">
+      <c r="N84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="O84" s="59">
+      <c r="O84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="P84" s="59">
+      <c r="P84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="Q84" s="59">
+      <c r="Q84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="R84" s="59">
+      <c r="R84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="S84" s="59">
+      <c r="S84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="T84" s="59">
+      <c r="T84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="U84" s="59">
+      <c r="U84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="V84" s="59">
+      <c r="V84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="W84" s="59">
+      <c r="W84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="X84" s="59">
+      <c r="X84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="Y84" s="59">
+      <c r="Y84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="Z84" s="59">
+      <c r="Z84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="AA84" s="59">
+      <c r="AA84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="AB84" s="59">
+      <c r="AB84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="AC84" s="59">
+      <c r="AC84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="AD84" s="59">
+      <c r="AD84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="AE84" s="59">
+      <c r="AE84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="AF84" s="59">
+      <c r="AF84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="AG84" s="59">
+      <c r="AG84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="AH84" s="59">
+      <c r="AH84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="AI84" s="59">
+      <c r="AI84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="AJ84" s="59">
+      <c r="AJ84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="AK84" s="59">
+      <c r="AK84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="AL84" s="59">
+      <c r="AL84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="AM84" s="59">
+      <c r="AM84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="AN84" s="59">
+      <c r="AN84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="AO84" s="59">
+      <c r="AO84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="AP84" s="59">
+      <c r="AP84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="AQ84" s="59">
+      <c r="AQ84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="AR84" s="59">
+      <c r="AR84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="AS84" s="59">
+      <c r="AS84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="AT84" s="59">
+      <c r="AT84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="AU84" s="59">
+      <c r="AU84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="AV84" s="59">
+      <c r="AV84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="AW84" s="59">
+      <c r="AW84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="AX84" s="59">
+      <c r="AX84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="AY84" s="59">
+      <c r="AY84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="AZ84" s="59">
+      <c r="AZ84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="BA84" s="59">
+      <c r="BA84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="BB84" s="59">
+      <c r="BB84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="BC84" s="59">
+      <c r="BC84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="BD84" s="59">
+      <c r="BD84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="BE84" s="59">
+      <c r="BE84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="BF84" s="59">
+      <c r="BF84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="BG84" s="59">
+      <c r="BG84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="BH84" s="59">
+      <c r="BH84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="BI84" s="59">
+      <c r="BI84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="BJ84" s="59">
+      <c r="BJ84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="BK84" s="59">
+      <c r="BK84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="BL84" s="59">
+      <c r="BL84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="BM84" s="59">
+      <c r="BM84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="BN84" s="59">
+      <c r="BN84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="BO84" s="59">
+      <c r="BO84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="BP84" s="59">
+      <c r="BP84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
-      <c r="BQ84" s="59">
+      <c r="BQ84" s="54">
         <f t="shared" si="92"/>
         <v>14.166666666666666</v>
       </c>
     </row>
-    <row r="85" spans="5:69" x14ac:dyDescent="0.25">
-      <c r="E85" s="59">
+    <row r="85" spans="4:69" x14ac:dyDescent="0.25">
+      <c r="D85" t="s">
+        <v>88</v>
+      </c>
+      <c r="E85" s="54">
         <f t="shared" si="91"/>
         <v>38.844999999999999</v>
       </c>
-      <c r="F85" s="59">
+      <c r="F85" s="54">
         <f t="shared" si="92"/>
         <v>38.844999999999999</v>
       </c>
-      <c r="G85" s="59">
+      <c r="G85" s="54">
         <f t="shared" si="92"/>
         <v>38.844999999999999</v>
       </c>
-      <c r="H85" s="59">
+      <c r="H85" s="54">
         <f t="shared" si="92"/>
         <v>38.844999999999999</v>
       </c>
-      <c r="I85" s="59">
+      <c r="I85" s="54">
         <f t="shared" si="92"/>
         <v>38.844999999999999</v>
       </c>
-      <c r="J85" s="59">
+      <c r="J85" s="54">
         <f t="shared" si="92"/>
         <v>38.844999999999999</v>
       </c>
-      <c r="K85" s="59">
+      <c r="K85" s="54">
         <f t="shared" si="92"/>
         <v>38.844999999999999</v>
       </c>
-      <c r="L85" s="59">
+      <c r="L85" s="54">
         <f t="shared" si="92"/>
         <v>38.844999999999999</v>
       </c>
-      <c r="M85" s="59">
+      <c r="M85" s="54">
         <f t="shared" si="92"/>
         <v>38.844999999999999</v>
       </c>
-      <c r="N85" s="59">
+      <c r="N85" s="54">
         <f t="shared" si="92"/>
         <v>38.844999999999999</v>
       </c>
-      <c r="O85" s="59">
+      <c r="O85" s="54">
         <f t="shared" si="92"/>
         <v>38.844999999999999</v>
       </c>
-      <c r="P85" s="59">
+      <c r="P85" s="54">
         <f t="shared" si="92"/>
         <v>38.844999999999999</v>
       </c>
-      <c r="Q85" s="59">
+      <c r="Q85" s="54">
         <f t="shared" si="92"/>
         <v>38.844999999999999</v>
       </c>
-      <c r="R85" s="59">
+      <c r="R85" s="54">
         <f t="shared" si="92"/>
         <v>38.844999999999999</v>
       </c>
-      <c r="S85" s="59">
+      <c r="S85" s="54">
         <f t="shared" si="92"/>
         <v>38.844999999999999</v>
       </c>
-      <c r="T85" s="59">
+      <c r="T85" s="54">
         <f t="shared" si="92"/>
         <v>38.844999999999999</v>
       </c>
-      <c r="U85" s="59">
+      <c r="U85" s="54">
         <f t="shared" si="92"/>
         <v>38.844999999999999</v>
       </c>
-      <c r="V85" s="59">
+      <c r="V85" s="54">
         <f t="shared" si="92"/>
         <v>38.844999999999999</v>
       </c>
-      <c r="W85" s="59">
+      <c r="W85" s="54">
         <f t="shared" si="92"/>
         <v>38.844999999999999</v>
       </c>
-      <c r="X85" s="59">
+      <c r="X85" s="54">
         <f t="shared" si="92"/>
         <v>38.844999999999999</v>
       </c>
-      <c r="Y85" s="59">
+      <c r="Y85" s="54">
         <f t="shared" si="92"/>
         <v>20.484999999999999</v>
       </c>
-      <c r="Z85" s="59">
+      <c r="Z85" s="54">
         <f t="shared" si="92"/>
         <v>20.484999999999999</v>
       </c>
-      <c r="AA85" s="59">
+      <c r="AA85" s="54">
         <f t="shared" si="92"/>
         <v>20.484999999999999</v>
       </c>
-      <c r="AB85" s="59">
+      <c r="AB85" s="54">
         <f t="shared" si="92"/>
         <v>20.484999999999999</v>
       </c>
-      <c r="AC85" s="59">
+      <c r="AC85" s="54">
         <f t="shared" si="92"/>
         <v>20.484999999999999</v>
       </c>
-      <c r="AD85" s="59">
+      <c r="AD85" s="54">
         <f t="shared" si="92"/>
         <v>20.484999999999999</v>
       </c>
-      <c r="AE85" s="59">
+      <c r="AE85" s="54">
         <f t="shared" si="92"/>
         <v>20.484999999999999</v>
       </c>
-      <c r="AF85" s="59">
+      <c r="AF85" s="54">
         <f t="shared" si="92"/>
         <v>20.484999999999999</v>
       </c>
-      <c r="AG85" s="59">
+      <c r="AG85" s="54">
         <f t="shared" si="92"/>
         <v>20.484999999999999</v>
       </c>
-      <c r="AH85" s="59">
+      <c r="AH85" s="54">
         <f t="shared" si="92"/>
         <v>20.484999999999999</v>
       </c>
-      <c r="AI85" s="59">
+      <c r="AI85" s="54">
         <f t="shared" si="92"/>
         <v>20.484999999999999</v>
       </c>
-      <c r="AJ85" s="59">
+      <c r="AJ85" s="54">
         <f t="shared" si="92"/>
         <v>20.484999999999999</v>
       </c>
-      <c r="AK85" s="59">
+      <c r="AK85" s="54">
         <f t="shared" si="92"/>
         <v>20.484999999999999</v>
       </c>
-      <c r="AL85" s="59">
+      <c r="AL85" s="54">
         <f t="shared" si="92"/>
         <v>20.484999999999999</v>
       </c>
-      <c r="AM85" s="59">
+      <c r="AM85" s="54">
         <f t="shared" si="92"/>
         <v>20.484999999999999</v>
       </c>
-      <c r="AN85" s="59">
+      <c r="AN85" s="54">
         <f t="shared" si="92"/>
         <v>20.484999999999999</v>
       </c>
-      <c r="AO85" s="59">
+      <c r="AO85" s="54">
         <f t="shared" si="92"/>
         <v>20.484999999999999</v>
       </c>
-      <c r="AP85" s="59">
+      <c r="AP85" s="54">
         <f t="shared" si="92"/>
         <v>20.484999999999999</v>
       </c>
-      <c r="AQ85" s="59">
+      <c r="AQ85" s="54">
         <f t="shared" si="92"/>
         <v>20.484999999999999</v>
       </c>
-      <c r="AR85" s="59">
+      <c r="AR85" s="54">
         <f t="shared" si="92"/>
         <v>20.484999999999999</v>
       </c>
-      <c r="AS85" s="59">
+      <c r="AS85" s="54">
         <f t="shared" si="92"/>
         <v>12.58</v>
       </c>
-      <c r="AT85" s="59">
+      <c r="AT85" s="54">
         <f t="shared" si="92"/>
         <v>12.58</v>
       </c>
-      <c r="AU85" s="59">
+      <c r="AU85" s="54">
         <f t="shared" si="92"/>
         <v>12.58</v>
       </c>
-      <c r="AV85" s="59">
+      <c r="AV85" s="54">
         <f t="shared" si="92"/>
         <v>12.58</v>
       </c>
-      <c r="AW85" s="59">
+      <c r="AW85" s="54">
         <f t="shared" si="92"/>
         <v>12.58</v>
       </c>
-      <c r="AX85" s="59">
+      <c r="AX85" s="54">
         <f t="shared" si="92"/>
         <v>12.58</v>
       </c>
-      <c r="AY85" s="59">
+      <c r="AY85" s="54">
         <f t="shared" si="92"/>
         <v>12.58</v>
       </c>
-      <c r="AZ85" s="59">
+      <c r="AZ85" s="54">
         <f t="shared" si="92"/>
         <v>12.58</v>
       </c>
-      <c r="BA85" s="59">
+      <c r="BA85" s="54">
         <f t="shared" si="92"/>
         <v>12.58</v>
       </c>
-      <c r="BB85" s="59">
+      <c r="BB85" s="54">
         <f t="shared" si="92"/>
         <v>12.58</v>
       </c>
-      <c r="BC85" s="59">
+      <c r="BC85" s="54">
         <f t="shared" si="92"/>
         <v>12.58</v>
       </c>
-      <c r="BD85" s="59">
+      <c r="BD85" s="54">
         <f t="shared" si="92"/>
         <v>12.58</v>
       </c>
-      <c r="BE85" s="59">
+      <c r="BE85" s="54">
         <f t="shared" si="92"/>
         <v>12.58</v>
       </c>
-      <c r="BF85" s="59">
+      <c r="BF85" s="54">
         <f t="shared" si="92"/>
         <v>12.58</v>
       </c>
-      <c r="BG85" s="59">
+      <c r="BG85" s="54">
         <f t="shared" si="92"/>
         <v>12.58</v>
       </c>
-      <c r="BH85" s="59">
+      <c r="BH85" s="54">
         <f t="shared" si="92"/>
         <v>12.58</v>
       </c>
-      <c r="BI85" s="59">
+      <c r="BI85" s="54">
         <f t="shared" si="92"/>
         <v>12.58</v>
       </c>
-      <c r="BJ85" s="59">
+      <c r="BJ85" s="54">
         <f t="shared" si="92"/>
         <v>12.58</v>
       </c>
-      <c r="BK85" s="59">
+      <c r="BK85" s="54">
         <f t="shared" si="92"/>
         <v>12.58</v>
       </c>
-      <c r="BL85" s="59">
+      <c r="BL85" s="54">
         <f t="shared" si="92"/>
         <v>12.58</v>
       </c>
-      <c r="BM85" s="59">
+      <c r="BM85" s="54">
         <f t="shared" si="92"/>
         <v>12.58</v>
       </c>
-      <c r="BN85" s="59">
+      <c r="BN85" s="54">
         <f t="shared" si="92"/>
         <v>12.58</v>
       </c>
-      <c r="BO85" s="59">
+      <c r="BO85" s="54">
         <f t="shared" si="92"/>
         <v>12.58</v>
       </c>
-      <c r="BP85" s="59">
+      <c r="BP85" s="54">
         <f t="shared" si="92"/>
         <v>12.58</v>
       </c>
-      <c r="BQ85" s="59">
+      <c r="BQ85" s="54">
         <f t="shared" si="92"/>
         <v>12.58</v>
       </c>
     </row>
-    <row r="86" spans="5:69" x14ac:dyDescent="0.25">
-      <c r="E86" s="59">
+    <row r="86" spans="4:69" x14ac:dyDescent="0.25">
+      <c r="D86" t="s">
+        <v>89</v>
+      </c>
+      <c r="E86" s="54">
         <f t="shared" si="91"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="F86" s="59">
+      <c r="F86" s="54">
         <f t="shared" si="92"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="G86" s="59">
+      <c r="G86" s="54">
         <f t="shared" si="92"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="H86" s="59">
+      <c r="H86" s="54">
         <f t="shared" si="92"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="I86" s="59">
+      <c r="I86" s="54">
         <f t="shared" si="92"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="J86" s="59">
+      <c r="J86" s="54">
         <f t="shared" si="92"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="K86" s="59">
+      <c r="K86" s="54">
         <f t="shared" si="92"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="L86" s="59">
+      <c r="L86" s="54">
         <f t="shared" si="92"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="M86" s="59">
+      <c r="M86" s="54">
         <f t="shared" si="92"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="N86" s="59">
+      <c r="N86" s="54">
         <f t="shared" si="92"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="O86" s="59">
+      <c r="O86" s="54">
         <f t="shared" si="92"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="P86" s="59">
+      <c r="P86" s="54">
         <f t="shared" si="92"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="Q86" s="59">
+      <c r="Q86" s="54">
         <f t="shared" si="92"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="R86" s="59">
+      <c r="R86" s="54">
         <f t="shared" si="92"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="S86" s="59">
+      <c r="S86" s="54">
         <f t="shared" ref="F86:BQ87" si="93">+S74*$C$78</f>
         <v>18.274999999999999</v>
       </c>
-      <c r="T86" s="59">
+      <c r="T86" s="54">
         <f t="shared" si="93"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="U86" s="59">
+      <c r="U86" s="54">
         <f t="shared" si="93"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="V86" s="59">
+      <c r="V86" s="54">
         <f t="shared" si="93"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="W86" s="59">
+      <c r="W86" s="54">
         <f t="shared" si="93"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="X86" s="59">
+      <c r="X86" s="54">
         <f t="shared" si="93"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="Y86" s="59">
+      <c r="Y86" s="54">
         <f t="shared" si="93"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="Z86" s="59">
+      <c r="Z86" s="54">
         <f t="shared" si="93"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="AA86" s="59">
+      <c r="AA86" s="54">
         <f t="shared" si="93"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="AB86" s="59">
+      <c r="AB86" s="54">
         <f t="shared" si="93"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="AC86" s="59">
+      <c r="AC86" s="54">
         <f t="shared" si="93"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="AD86" s="59">
+      <c r="AD86" s="54">
         <f t="shared" si="93"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="AE86" s="59">
+      <c r="AE86" s="54">
         <f t="shared" si="93"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="AF86" s="59">
+      <c r="AF86" s="54">
         <f t="shared" si="93"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="AG86" s="59">
+      <c r="AG86" s="54">
         <f t="shared" si="93"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="AH86" s="59">
+      <c r="AH86" s="54">
         <f t="shared" si="93"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="AI86" s="59">
+      <c r="AI86" s="54">
         <f t="shared" si="93"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="AJ86" s="59">
+      <c r="AJ86" s="54">
         <f t="shared" si="93"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="AK86" s="59">
+      <c r="AK86" s="54">
         <f t="shared" si="93"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="AL86" s="59">
+      <c r="AL86" s="54">
         <f t="shared" si="93"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="AM86" s="59">
+      <c r="AM86" s="54">
         <f t="shared" si="93"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="AN86" s="59">
+      <c r="AN86" s="54">
         <f t="shared" si="93"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="AO86" s="59">
+      <c r="AO86" s="54">
         <f t="shared" si="93"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="AP86" s="59">
+      <c r="AP86" s="54">
         <f t="shared" si="93"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="AQ86" s="59">
+      <c r="AQ86" s="54">
         <f t="shared" si="93"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="AR86" s="59">
+      <c r="AR86" s="54">
         <f t="shared" si="93"/>
         <v>18.274999999999999</v>
       </c>
-      <c r="AS86" s="59">
+      <c r="AS86" s="54">
         <f t="shared" si="93"/>
         <v>15.98</v>
       </c>
-      <c r="AT86" s="59">
+      <c r="AT86" s="54">
         <f t="shared" si="93"/>
         <v>15.98</v>
       </c>
-      <c r="AU86" s="59">
+      <c r="AU86" s="54">
         <f t="shared" si="93"/>
         <v>15.98</v>
       </c>
-      <c r="AV86" s="59">
+      <c r="AV86" s="54">
         <f t="shared" si="93"/>
         <v>15.98</v>
       </c>
-      <c r="AW86" s="59">
+      <c r="AW86" s="54">
         <f t="shared" si="93"/>
         <v>15.98</v>
       </c>
-      <c r="AX86" s="59">
+      <c r="AX86" s="54">
         <f t="shared" si="93"/>
         <v>15.98</v>
       </c>
-      <c r="AY86" s="59">
+      <c r="AY86" s="54">
         <f t="shared" si="93"/>
         <v>15.98</v>
       </c>
-      <c r="AZ86" s="59">
+      <c r="AZ86" s="54">
         <f t="shared" si="93"/>
         <v>15.98</v>
       </c>
-      <c r="BA86" s="59">
+      <c r="BA86" s="54">
         <f t="shared" si="93"/>
         <v>15.98</v>
       </c>
-      <c r="BB86" s="59">
+      <c r="BB86" s="54">
         <f t="shared" si="93"/>
         <v>15.98</v>
       </c>
-      <c r="BC86" s="59">
+      <c r="BC86" s="54">
         <f t="shared" si="93"/>
         <v>15.98</v>
       </c>
-      <c r="BD86" s="59">
+      <c r="BD86" s="54">
         <f t="shared" si="93"/>
         <v>15.98</v>
       </c>
-      <c r="BE86" s="59">
+      <c r="BE86" s="54">
         <f t="shared" si="93"/>
         <v>15.98</v>
       </c>
-      <c r="BF86" s="59">
+      <c r="BF86" s="54">
         <f t="shared" si="93"/>
         <v>15.98</v>
       </c>
-      <c r="BG86" s="59">
+      <c r="BG86" s="54">
         <f t="shared" si="93"/>
         <v>15.98</v>
       </c>
-      <c r="BH86" s="59">
+      <c r="BH86" s="54">
         <f t="shared" si="93"/>
         <v>15.98</v>
       </c>
-      <c r="BI86" s="59">
+      <c r="BI86" s="54">
         <f t="shared" si="93"/>
         <v>15.98</v>
       </c>
-      <c r="BJ86" s="59">
+      <c r="BJ86" s="54">
         <f t="shared" si="93"/>
         <v>15.98</v>
       </c>
-      <c r="BK86" s="59">
+      <c r="BK86" s="54">
         <f t="shared" si="93"/>
         <v>15.98</v>
       </c>
-      <c r="BL86" s="59">
+      <c r="BL86" s="54">
         <f t="shared" si="93"/>
         <v>15.98</v>
       </c>
-      <c r="BM86" s="59">
+      <c r="BM86" s="54">
         <f t="shared" si="93"/>
         <v>15.98</v>
       </c>
-      <c r="BN86" s="59">
+      <c r="BN86" s="54">
         <f t="shared" si="93"/>
         <v>15.98</v>
       </c>
-      <c r="BO86" s="59">
+      <c r="BO86" s="54">
         <f t="shared" si="93"/>
         <v>15.98</v>
       </c>
-      <c r="BP86" s="59">
+      <c r="BP86" s="54">
         <f t="shared" si="93"/>
         <v>15.98</v>
       </c>
-      <c r="BQ86" s="59">
+      <c r="BQ86" s="54">
         <f t="shared" si="93"/>
         <v>15.98</v>
       </c>
     </row>
-    <row r="87" spans="5:69" x14ac:dyDescent="0.25">
-      <c r="E87" s="59">
+    <row r="87" spans="4:69" x14ac:dyDescent="0.25">
+      <c r="D87" t="s">
+        <v>12</v>
+      </c>
+      <c r="E87" s="54">
         <f t="shared" si="91"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="F87" s="59">
+      <c r="F87" s="54">
         <f t="shared" si="93"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="G87" s="59">
+      <c r="G87" s="54">
         <f t="shared" si="93"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="H87" s="59">
+      <c r="H87" s="54">
         <f t="shared" si="93"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="I87" s="59">
+      <c r="I87" s="54">
         <f t="shared" si="93"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="J87" s="59">
+      <c r="J87" s="54">
         <f t="shared" si="93"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="K87" s="59">
+      <c r="K87" s="54">
         <f t="shared" si="93"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="L87" s="59">
+      <c r="L87" s="54">
         <f t="shared" si="93"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="M87" s="59">
+      <c r="M87" s="54">
         <f t="shared" si="93"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="N87" s="59">
+      <c r="N87" s="54">
         <f t="shared" si="93"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="O87" s="59">
+      <c r="O87" s="54">
         <f t="shared" si="93"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="P87" s="59">
+      <c r="P87" s="54">
         <f t="shared" si="93"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="Q87" s="59">
+      <c r="Q87" s="54">
         <f t="shared" si="93"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="R87" s="59">
+      <c r="R87" s="54">
         <f t="shared" si="93"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="S87" s="59">
+      <c r="S87" s="54">
         <f t="shared" si="93"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="T87" s="59">
+      <c r="T87" s="54">
         <f t="shared" si="93"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="U87" s="59">
+      <c r="U87" s="54">
         <f t="shared" si="93"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="V87" s="59">
+      <c r="V87" s="54">
         <f t="shared" si="93"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="W87" s="59">
+      <c r="W87" s="54">
         <f t="shared" si="93"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="X87" s="59">
+      <c r="X87" s="54">
         <f t="shared" si="93"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="Y87" s="59">
+      <c r="Y87" s="54">
         <f t="shared" si="93"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="Z87" s="59">
+      <c r="Z87" s="54">
         <f t="shared" si="93"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="AA87" s="59">
+      <c r="AA87" s="54">
         <f t="shared" si="93"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="AB87" s="59">
+      <c r="AB87" s="54">
         <f t="shared" si="93"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="AC87" s="59">
+      <c r="AC87" s="54">
         <f t="shared" si="93"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="AD87" s="59">
+      <c r="AD87" s="54">
         <f t="shared" si="93"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="AE87" s="59">
+      <c r="AE87" s="54">
         <f t="shared" si="93"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="AF87" s="59">
+      <c r="AF87" s="54">
         <f t="shared" si="93"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="AG87" s="59">
+      <c r="AG87" s="54">
         <f t="shared" si="93"/>
         <v>8.3333333333333339</v>
       </c>
-      <c r="AH87" s="59">
+      <c r="AH87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="AI87" s="59">
+      <c r="AI87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="AJ87" s="59">
+      <c r="AJ87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="AK87" s="59">
+      <c r="AK87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="AL87" s="59">
+      <c r="AL87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="AM87" s="59">
+      <c r="AM87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="AN87" s="59">
+      <c r="AN87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="AO87" s="59">
+      <c r="AO87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="AP87" s="59">
+      <c r="AP87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="AQ87" s="59">
+      <c r="AQ87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="AR87" s="59">
+      <c r="AR87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="AS87" s="59">
+      <c r="AS87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="AT87" s="59">
+      <c r="AT87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="AU87" s="59">
+      <c r="AU87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="AV87" s="59">
+      <c r="AV87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="AW87" s="59">
+      <c r="AW87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="AX87" s="59">
+      <c r="AX87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="AY87" s="59">
+      <c r="AY87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="AZ87" s="59">
+      <c r="AZ87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="BA87" s="59">
+      <c r="BA87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="BB87" s="59">
+      <c r="BB87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="BC87" s="59">
+      <c r="BC87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="BD87" s="59">
+      <c r="BD87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="BE87" s="59">
+      <c r="BE87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="BF87" s="59">
+      <c r="BF87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="BG87" s="59">
+      <c r="BG87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="BH87" s="59">
+      <c r="BH87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="BI87" s="59">
+      <c r="BI87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="BJ87" s="59">
+      <c r="BJ87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="BK87" s="59">
+      <c r="BK87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="BL87" s="59">
+      <c r="BL87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="BM87" s="59">
+      <c r="BM87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="BN87" s="59">
+      <c r="BN87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="BO87" s="59">
+      <c r="BO87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="BP87" s="59">
+      <c r="BP87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>
-      <c r="BQ87" s="59">
+      <c r="BQ87" s="54">
         <f t="shared" si="93"/>
         <v>5.5555555555555554</v>
       </c>

</xml_diff>